<commit_message>
Completed Add Product flow :- QA-606
</commit_message>
<xml_diff>
--- a/binaries/CGFiles/ChannelGateTestData.xlsx
+++ b/binaries/CGFiles/ChannelGateTestData.xlsx
@@ -2,22 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13860" windowHeight="6330"/>
+    <workbookView activeTab="1" windowHeight="6330" windowWidth="13860" xWindow="0" yWindow="2520"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Add Product" r:id="rId2" sheetId="2"/>
+    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="101">
   <si>
     <t>Useremail</t>
   </si>
@@ -38,13 +37,296 @@
   </si>
   <si>
     <t>Test123!</t>
+  </si>
+  <si>
+    <t>Product Title</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Collections</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Test 3</t>
+  </si>
+  <si>
+    <t>Abbington</t>
+  </si>
+  <si>
+    <t>Baby / Baby Furniture / Baby Bassinets</t>
+  </si>
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>UPC</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Wholesale</t>
+  </si>
+  <si>
+    <t>Country of Manufacture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAP </t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Beige</t>
+  </si>
+  <si>
+    <t>Cast Iron</t>
+  </si>
+  <si>
+    <t>Modern</t>
+  </si>
+  <si>
+    <t>Short Description</t>
+  </si>
+  <si>
+    <t>Feature 1</t>
+  </si>
+  <si>
+    <t>Feature 2</t>
+  </si>
+  <si>
+    <t>Feature 3</t>
+  </si>
+  <si>
+    <t>Available Quantity</t>
+  </si>
+  <si>
+    <t>Shipping Service</t>
+  </si>
+  <si>
+    <t>Min Lead Time</t>
+  </si>
+  <si>
+    <t>Max Lead Time</t>
+  </si>
+  <si>
+    <t>HS Code</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Qty </t>
+  </si>
+  <si>
+    <t>Package Type</t>
+  </si>
+  <si>
+    <t>Package SKU</t>
+  </si>
+  <si>
+    <t>Carton</t>
+  </si>
+  <si>
+    <t>283</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>913</t>
+  </si>
+  <si>
+    <t>534</t>
+  </si>
+  <si>
+    <t>An excellent example of transitional style, the London collection by Test features plush hand-rubbed Italian leather cushioning, classic brass nailhead trim, and the perfect merger of contemporary sleek lines with traditional sumptuous curves. Transitional pieces such as these compliment both classic and modern decors without overpowering either.</t>
+  </si>
+  <si>
+    <t>Kiln-dried solid hardwood frame</t>
+  </si>
+  <si>
+    <t>Tempered glass</t>
+  </si>
+  <si>
+    <t>Leather match on sides and back</t>
+  </si>
+  <si>
+    <t>Dining Table Dimensions</t>
+  </si>
+  <si>
+    <t>Table Leaf Dimensions</t>
+  </si>
+  <si>
+    <t>Table Weight</t>
+  </si>
+  <si>
+    <t>35.5"W x 0.75"D</t>
+  </si>
+  <si>
+    <t>43.3" H x 4.9" W x 43.3" D</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>CG/SKU/1-4</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>9403001050</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Freight</t>
+  </si>
+  <si>
+    <t>MSRP</t>
+  </si>
+  <si>
+    <t>Key1</t>
+  </si>
+  <si>
+    <t>Value1</t>
+  </si>
+  <si>
+    <t>Key2</t>
+  </si>
+  <si>
+    <t>Value2</t>
+  </si>
+  <si>
+    <t>Key3</t>
+  </si>
+  <si>
+    <t>Value3</t>
+  </si>
+  <si>
+    <t>Package Height</t>
+  </si>
+  <si>
+    <t>Package Width</t>
+  </si>
+  <si>
+    <t>Package Depth</t>
+  </si>
+  <si>
+    <t>Package Weight</t>
+  </si>
+  <si>
+    <t>Product Id</t>
+  </si>
+  <si>
+    <t>Net5-Check10</t>
+  </si>
+  <si>
+    <t>054132691452</t>
+  </si>
+  <si>
+    <t>2266776</t>
+  </si>
+  <si>
+    <t>Test Automation Title 10299</t>
+  </si>
+  <si>
+    <t>UPC2</t>
+  </si>
+  <si>
+    <t>UPC3</t>
+  </si>
+  <si>
+    <t>UPC4</t>
+  </si>
+  <si>
+    <t>987654321098</t>
+  </si>
+  <si>
+    <t>012000007897</t>
+  </si>
+  <si>
+    <t>036000291452</t>
+  </si>
+  <si>
+    <t>Test Automation Title 16</t>
+  </si>
+  <si>
+    <t>automation_sku_166</t>
+  </si>
+  <si>
+    <t>2266777</t>
+  </si>
+  <si>
+    <t>Test Automation Title 2453</t>
+  </si>
+  <si>
+    <t>Test Automation Title 96621</t>
+  </si>
+  <si>
+    <t>Test Automation Title 1629</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,16 +341,32 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -76,24 +374,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+  <cellXfs count="18">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="3" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -102,10 +444,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -261,7 +603,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -270,13 +612,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -286,7 +628,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -295,7 +637,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -304,7 +646,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -314,12 +656,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -350,7 +692,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -369,7 +711,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -382,17 +724,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -424,22 +766,321 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink r:id="rId1" ref="A2"/>
+    <hyperlink r:id="rId2" ref="A3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AS2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AQ5" sqref="AQ5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.4765625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="35.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.66015625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="2" width="61.5703125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="42" max="44" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:44">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row ht="90" r="2" spans="1:44">
+      <c r="A2" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AI2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AQ2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR2" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -451,6 +1092,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Reroute request scripts
</commit_message>
<xml_diff>
--- a/binaries/CGFiles/ChannelGateTestData.xlsx
+++ b/binaries/CGFiles/ChannelGateTestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="149">
   <si>
     <t>Useremail</t>
   </si>
@@ -430,6 +430,39 @@
   </si>
   <si>
     <t>2350957</t>
+  </si>
+  <si>
+    <t>automation_sku_204</t>
+  </si>
+  <si>
+    <t>Test Automation Title 32776</t>
+  </si>
+  <si>
+    <t>Test Automation Title 20</t>
+  </si>
+  <si>
+    <t>automation_sku_455</t>
+  </si>
+  <si>
+    <t>Test Automation Title 12</t>
+  </si>
+  <si>
+    <t>automation_sku_794</t>
+  </si>
+  <si>
+    <t>Test Automation Title 57935</t>
+  </si>
+  <si>
+    <t>Test Automation Title 13</t>
+  </si>
+  <si>
+    <t>automation_sku_969</t>
+  </si>
+  <si>
+    <t>2389173</t>
+  </si>
+  <si>
+    <t>Test Automation Title 1209</t>
   </si>
 </sst>
 </file>
@@ -532,7 +565,7 @@
     </xf>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
@@ -557,6 +590,19 @@
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" quotePrefix="1" xfId="2"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
@@ -1084,11 +1130,11 @@
       </c>
     </row>
     <row ht="90" r="2" spans="1:44">
-      <c r="A2" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>137</v>
+      <c r="A2" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>147</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>11</v>
@@ -1099,8 +1145,8 @@
       <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="21" t="s">
-        <v>135</v>
+      <c r="F2" s="33" t="s">
+        <v>146</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>85</v>

</xml_diff>